<commit_message>
Added Time Logs testcases
a. Created 2 Time Logs TestCases
b. edited Homepage
c. Added EditTimeLogs
</commit_message>
<xml_diff>
--- a/testData_arch/timetracker_glenn_v2.xlsx
+++ b/testData_arch/timetracker_glenn_v2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">TC001_TimeTracker_TimeLogs_LogTimeIn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC002_TimeTracker_TimeLogs_LogTimeOut</t>
   </si>
 </sst>
 </file>
@@ -355,7 +358,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,10 +387,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Finished TimeLogs and started ChargeHours
Time Logs
a. Finished all TimeLog test cases
b. Added new error verifications and actions in EditTimeLogs page
c. improved code readability

DailyWorkHours
a. created new DailyWorkHours page
b. finished 3 TCs under ChargeHours

Misc
a. added burner .java file to run test code before application to test case
b. created additional xml file to run all testcases
c. updated test data on excel file
</commit_message>
<xml_diff>
--- a/testData_arch/timetracker_glenn_v2.xlsx
+++ b/testData_arch/timetracker_glenn_v2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="27">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -70,13 +70,40 @@
     <t xml:space="preserve">timein</t>
   </si>
   <si>
-    <t xml:space="preserve">timout</t>
+    <t xml:space="preserve">timeout</t>
   </si>
   <si>
     <t xml:space="preserve">TC001_TimeTracker_TimeLogs_LogTimeIn</t>
   </si>
   <si>
     <t xml:space="preserve">TC002_TimeTracker_TimeLogs_LogTimeOut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC003_TimeTracker_TimeLogs_EqualTimeInTimeOut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC004_TimeTracker_TimeLogs_TimeInLaterThanTimeOut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC005_TimeTracker_TimeLogs_ReasonNull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC006_TimeTracker_TimeLogs_LogValidTimeInTimeOut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC007_Timetracker_TimeLogs_CancelTimeInTimeOut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC001_TimeTracker_ChargeHours_ClickInputWhizHours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC001_TimeTracker_ChargeHours_ClickInputWhizHour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC002_TimeTracker_ChargeHours_DailyWorkHoursCloseButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC003_TimeTracker_ChargeHours_DailyWorkHoursDateDisplayed</t>
   </si>
 </sst>
 </file>
@@ -113,16 +140,16 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -169,7 +196,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,6 +209,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,20 +221,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -226,7 +257,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -294,6 +325,8 @@
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -398,17 +431,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="51.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,7 +454,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -461,32 +494,75 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -508,68 +584,71 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.2"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -592,69 +671,78 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.62"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
+      <c r="A4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
+      <c r="B5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="9" t="s">
         <v>12</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of changes, finished Charge Hours
pageObjects
- added more comments for easier readability
- added InputWhizHours functions, selecting tasks, fill up fields, and verify entered data

TimeLogs
- optimized code for easier readability and

ChargeHours
- finished TC004 to TC022

Misc
- added ForTestingIdeas.java for running simple code snippets
</commit_message>
<xml_diff>
--- a/testData_arch/timetracker_glenn_v2.xlsx
+++ b/testData_arch/timetracker_glenn_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="52">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -73,9 +73,15 @@
     <t xml:space="preserve">timeout</t>
   </si>
   <si>
+    <t xml:space="preserve">remarks</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC001_TimeTracker_TimeLogs_LogTimeIn</t>
   </si>
   <si>
+    <t xml:space="preserve">automated fillup by Selenium</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC002_TimeTracker_TimeLogs_LogTimeOut</t>
   </si>
   <si>
@@ -97,13 +103,82 @@
     <t xml:space="preserve">TC001_TimeTracker_ChargeHours_ClickInputWhizHours</t>
   </si>
   <si>
-    <t xml:space="preserve">TC001_TimeTracker_ChargeHours_ClickInputWhizHour</t>
+    <t xml:space="preserve">project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">milestone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taskname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actualHours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">typeOfWork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jensen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JFC Tosca - Training and Training Prep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General Tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal</t>
   </si>
   <si>
     <t xml:space="preserve">TC002_TimeTracker_ChargeHours_DailyWorkHoursCloseButton</t>
   </si>
   <si>
     <t xml:space="preserve">TC003_TimeTracker_ChargeHours_DailyWorkHoursDateDisplayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC004_TimeTracker_ChargeHours_DailyWorkHoursProjectsDropdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC005_TimeTracker_ChargeHours_DailyWorkHours_DeliverableMilestone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC014_TimeTracker_ChargeHours_DailyWorkHours_AllTasksTasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Tasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC015_TimeTracker_ChargeHours_DailyWorkHours_GeneralTasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC016_TimeTracker_ChargeHours_DailyWorkHours_GeneralTasksTasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC017_TimeTracker_ChargeHours_DailyWorkHours_AllocatedHours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC018_TimeTracker_ChargeHours_DailyWorkHours_ActualWorkHoursNumberOfHours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC019_TimeTracker_ChargeHours_DailyWorkHours_ActualWorkHoursTypeOfWork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OverTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC020_TimeTracker_ChargeHours_DailyWorkHours_ActualWorkHoursDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC021_TimeTracker_ChargeHours_DailyWorkHours_ActualWorkHoursSaveButton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC022_TimeTracker_ChargeHours_DailyWorkHours_ActualHoursAndLoggedHours</t>
   </si>
 </sst>
 </file>
@@ -116,7 +191,7 @@
     <numFmt numFmtId="166" formatCode="h:mm\ AM/PM"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -150,6 +225,13 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -196,7 +278,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,6 +319,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -257,7 +343,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,10 +517,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -463,10 +549,13 @@
       <c r="F1" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -483,10 +572,13 @@
       <c r="F2" s="7" t="n">
         <v>0.708333333333333</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -494,13 +586,22 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="8" t="n">
+        <v>45071</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -508,13 +609,22 @@
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
+      <c r="D4" s="8" t="n">
+        <v>45071</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -522,13 +632,22 @@
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="8" t="n">
+        <v>45071</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -536,13 +655,22 @@
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+      <c r="D6" s="8" t="n">
+        <v>45071</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -550,19 +678,40 @@
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="D7" s="8" t="n">
+        <v>45071</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>45071</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -605,7 +754,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>4</v>
@@ -668,15 +817,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="10" width="57.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,60 +839,474 @@
       <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>